<commit_message>
new branch and content
</commit_message>
<xml_diff>
--- a/Brutal Assault Schedule.xlsx
+++ b/Brutal Assault Schedule.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://twodegrees1-my.sharepoint.com/personal/michal_sicak_slalom_com/Documents/Datapun/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\___Projects\Python\.python_virtual_environments\Brutal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="245" yWindow="109" windowWidth="14808" windowHeight="8015"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bands" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Attendance!$A$1:$E$23</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="310">
   <si>
     <t>Year</t>
   </si>
@@ -966,7 +966,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1319,19 +1319,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
+    <sheetView topLeftCell="A168" workbookViewId="0">
       <selection activeCell="F202" sqref="F202"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.625" customWidth="1"/>
-    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.75" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5610,19 +5610,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5938,6 +5938,9 @@
       <c r="C22" t="s">
         <v>159</v>
       </c>
+      <c r="D22">
+        <v>110</v>
+      </c>
       <c r="E22">
         <v>4</v>
       </c>
@@ -5952,8 +5955,25 @@
       <c r="C23" t="s">
         <v>159</v>
       </c>
+      <c r="D23">
+        <v>130</v>
+      </c>
       <c r="E23">
         <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2016</v>
+      </c>
+      <c r="B24">
+        <v>18000</v>
+      </c>
+      <c r="C24" t="s">
+        <v>159</v>
+      </c>
+      <c r="D24">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>